<commit_message>
feat: prev jl-set 2025
</commit_message>
<xml_diff>
--- a/data/datasets_produtos/ilheus/acucar_ilheus.xlsx
+++ b/data/datasets_produtos/ilheus/acucar_ilheus.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Meus Codes\previsao_cestas\data\datasets_produtos\ilheus\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079D165F-3586-4C14-A956-253DC4764E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="acucar_ilheus" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="acucar_ilheus" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
   <si>
     <t>ano</t>
   </si>
@@ -334,23 +351,26 @@
   </si>
   <si>
     <t>31-04-2025</t>
+  </si>
+  <si>
+    <t>31-06-2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.000000"/>
+      <sz val="10"/>
       <color indexed="64"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.000000"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -364,28 +384,28 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,291 +423,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -890,26 +627,27 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="0" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B247"/>
   <sheetViews>
-    <sheetView topLeftCell="A220" zoomScale="100" workbookViewId="0">
-      <selection activeCell="B246" activeCellId="0" sqref="B246"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="B248" sqref="B248"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="1" width="14.42578125"/>
+    <col min="1" max="1" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -917,7 +655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>38383</v>
       </c>
@@ -925,7 +663,7 @@
         <v>3.21</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -933,15 +671,15 @@
         <v>3.21</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>38442</v>
       </c>
       <c r="B4" s="4">
-        <v>3.3900000000000001</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -949,63 +687,63 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>38503</v>
       </c>
       <c r="B6" s="4">
-        <v>3.4199999999999999</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
+        <v>3.42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="4">
-        <v>3.2400000000000002</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>38564</v>
       </c>
       <c r="B8" s="4">
-        <v>3.3900000000000001</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>38595</v>
       </c>
       <c r="B9" s="4">
-        <v>3.2400000000000002</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4">
-        <v>3.2999999999999998</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>38656</v>
       </c>
       <c r="B11" s="4">
-        <v>3.5099999999999998</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="4">
-        <v>3.6600000000000001</v>
-      </c>
-    </row>
-    <row r="13" ht="12.75">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>38717</v>
       </c>
@@ -1013,15 +751,15 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="14" ht="12.75">
+    <row r="14" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>38748</v>
       </c>
       <c r="B14" s="4">
-        <v>4.3799999999999999</v>
-      </c>
-    </row>
-    <row r="15" ht="12.75">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -1029,7 +767,7 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="16" ht="12.75">
+    <row r="16" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>38807</v>
       </c>
@@ -1037,47 +775,47 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="17" ht="12.75">
+    <row r="17" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="4">
-        <v>5.2800000000000002</v>
-      </c>
-    </row>
-    <row r="18" ht="12.75">
+        <v>5.28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>38868</v>
       </c>
       <c r="B18" s="4">
-        <v>5.3399999999999999</v>
-      </c>
-    </row>
-    <row r="19" ht="12.75">
+        <v>5.34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="4">
-        <v>5.3399999999999999</v>
-      </c>
-    </row>
-    <row r="20" ht="12.75">
+        <v>5.34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>38929</v>
       </c>
       <c r="B20" s="4">
-        <v>5.3399999999999999</v>
-      </c>
-    </row>
-    <row r="21" ht="12.75">
+        <v>5.34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>38960</v>
       </c>
       <c r="B21" s="4">
-        <v>5.3099999999999996</v>
-      </c>
-    </row>
-    <row r="22" ht="12.75">
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1085,7 +823,7 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="23" ht="12.75">
+    <row r="23" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>39021</v>
       </c>
@@ -1093,15 +831,15 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="24" ht="12.75">
+    <row r="24" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="4">
-        <v>4.3799999999999999</v>
-      </c>
-    </row>
-    <row r="25" ht="12.75">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>39082</v>
       </c>
@@ -1109,15 +847,15 @@
         <v>4.2300000000000004</v>
       </c>
     </row>
-    <row r="26" ht="12.75">
+    <row r="26" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>39113</v>
       </c>
       <c r="B26" s="4">
-        <v>4.1699999999999999</v>
-      </c>
-    </row>
-    <row r="27" ht="12.75">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
@@ -1125,31 +863,31 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="28" ht="12.75">
+    <row r="28" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>39172</v>
       </c>
       <c r="B28" s="4">
-        <v>4.1699999999999999</v>
-      </c>
-    </row>
-    <row r="29" ht="12.75">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="4">
-        <v>4.1699999999999999</v>
-      </c>
-    </row>
-    <row r="30" ht="12.75">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>39233</v>
       </c>
       <c r="B30" s="4">
-        <v>3.9300000000000002</v>
-      </c>
-    </row>
-    <row r="31" ht="12.75">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -1157,31 +895,31 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="32" ht="12.75">
+    <row r="32" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>39294</v>
       </c>
       <c r="B32" s="4">
-        <v>3.0600000000000001</v>
-      </c>
-    </row>
-    <row r="33" ht="12.75">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>39325</v>
       </c>
       <c r="B33" s="4">
-        <v>3.1499999999999999</v>
-      </c>
-    </row>
-    <row r="34" ht="12.75">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="4">
-        <v>3.0299999999999998</v>
-      </c>
-    </row>
-    <row r="35" ht="12.75">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>39386</v>
       </c>
@@ -1189,111 +927,111 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" ht="12.75">
+    <row r="36" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="4">
-        <v>2.8799999999999999</v>
-      </c>
-    </row>
-    <row r="37" ht="12.75">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>39447</v>
       </c>
       <c r="B37" s="4">
-        <v>2.9399999999999999</v>
-      </c>
-    </row>
-    <row r="38" ht="12.75">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>39478</v>
       </c>
       <c r="B38" s="4">
-        <v>3.0600000000000001</v>
-      </c>
-    </row>
-    <row r="39" ht="12.75">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B39" s="4">
-        <v>3.0600000000000001</v>
-      </c>
-    </row>
-    <row r="40" ht="12.75">
+        <v>3.06</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39538</v>
       </c>
       <c r="B40" s="4">
-        <v>3.2400000000000002</v>
-      </c>
-    </row>
-    <row r="41" ht="12.75">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B41" s="4">
-        <v>3.3599999999999999</v>
-      </c>
-    </row>
-    <row r="42" ht="12.75">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>39599</v>
       </c>
       <c r="B42" s="4">
-        <v>3.3599999999999999</v>
-      </c>
-    </row>
-    <row r="43" ht="12.75">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="4">
-        <v>3.3900000000000001</v>
-      </c>
-    </row>
-    <row r="44" ht="12.75">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>39660</v>
       </c>
       <c r="B44" s="4">
-        <v>3.1499999999999999</v>
-      </c>
-    </row>
-    <row r="45" ht="12.75">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>39691</v>
       </c>
       <c r="B45" s="4">
-        <v>3.2400000000000002</v>
-      </c>
-    </row>
-    <row r="46" ht="12.75">
+        <v>3.24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B46" s="4">
-        <v>3.2999999999999998</v>
-      </c>
-    </row>
-    <row r="47" ht="12.75">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>39752</v>
       </c>
       <c r="B47" s="4">
-        <v>3.3900000000000001</v>
-      </c>
-    </row>
-    <row r="48" ht="12.75">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B48" s="4">
-        <v>3.6000000000000001</v>
-      </c>
-    </row>
-    <row r="49" ht="12.75">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>39813</v>
       </c>
@@ -1301,7 +1039,7 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="50" ht="12.75">
+    <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>39844</v>
       </c>
@@ -1309,31 +1047,31 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="51" ht="12.75">
+    <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B51" s="4">
-        <v>4.6799999999999997</v>
-      </c>
-    </row>
-    <row r="52" ht="12.75">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>39903</v>
       </c>
       <c r="B52" s="4">
-        <v>4.9199999999999999</v>
-      </c>
-    </row>
-    <row r="53" ht="12.75">
+        <v>4.92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="4">
-        <v>5.0099999999999998</v>
-      </c>
-    </row>
-    <row r="54" ht="12.75">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>39964</v>
       </c>
@@ -1341,7 +1079,7 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="55" ht="12.75">
+    <row r="55" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>24</v>
       </c>
@@ -1349,15 +1087,15 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="56" ht="12.75">
+    <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>40025</v>
       </c>
       <c r="B56" s="4">
-        <v>4.7400000000000002</v>
-      </c>
-    </row>
-    <row r="57" ht="12.75">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>40056</v>
       </c>
@@ -1365,15 +1103,15 @@
         <v>4.71</v>
       </c>
     </row>
-    <row r="58" ht="12.75">
+    <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B58" s="4">
-        <v>5.2199999999999998</v>
-      </c>
-    </row>
-    <row r="59" ht="12.75">
+        <v>5.22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>40117</v>
       </c>
@@ -1381,15 +1119,15 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="60" ht="12.75">
+    <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B60" s="4">
-        <v>5.2199999999999998</v>
-      </c>
-    </row>
-    <row r="61" ht="12.75">
+        <v>5.22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>40178</v>
       </c>
@@ -1397,207 +1135,207 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="62" ht="12.75">
+    <row r="62" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>40209</v>
       </c>
       <c r="B62" s="4">
-        <v>6.5999999999999996</v>
-      </c>
-    </row>
-    <row r="63" ht="12.75">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B63" s="4">
-        <v>6.7800000000000002</v>
-      </c>
-    </row>
-    <row r="64" ht="12.75">
+        <v>6.78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>40268</v>
       </c>
       <c r="B64" s="4">
-        <v>6.8399999999999999</v>
-      </c>
-    </row>
-    <row r="65" ht="12.75">
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B65" s="4">
-        <v>6.3899999999999997</v>
-      </c>
-    </row>
-    <row r="66" ht="12.75">
+        <v>6.39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>40329</v>
       </c>
       <c r="B66" s="4">
-        <v>6.2400000000000002</v>
-      </c>
-    </row>
-    <row r="67" ht="12.75">
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B67" s="4">
-        <v>5.7300000000000004</v>
-      </c>
-    </row>
-    <row r="68" ht="12.75">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>40390</v>
       </c>
       <c r="B68" s="4">
-        <v>5.0099999999999998</v>
-      </c>
-    </row>
-    <row r="69" ht="12.75">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>40421</v>
       </c>
       <c r="B69" s="4">
-        <v>4.8300000000000001</v>
-      </c>
-    </row>
-    <row r="70" ht="12.75">
+        <v>4.83</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B70" s="4">
-        <v>5.3099999999999996</v>
-      </c>
-    </row>
-    <row r="71" ht="12.75">
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>40482</v>
       </c>
       <c r="B71" s="4">
-        <v>6.0300000000000002</v>
-      </c>
-    </row>
-    <row r="72" ht="12.75">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B72" s="4">
-        <v>6.5999999999999996</v>
-      </c>
-    </row>
-    <row r="73" ht="12.75">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>40543</v>
       </c>
       <c r="B73" s="4">
-        <v>6.2999999999999998</v>
-      </c>
-    </row>
-    <row r="74" ht="12.75">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>40574</v>
       </c>
       <c r="B74" s="4">
-        <v>6.3899999999999997</v>
-      </c>
-    </row>
-    <row r="75" ht="12.75">
+        <v>6.39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B75" s="4">
-        <v>6.4500000000000002</v>
-      </c>
-    </row>
-    <row r="76" ht="12.75">
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>40633</v>
       </c>
       <c r="B76" s="4">
-        <v>6.4800000000000004</v>
-      </c>
-    </row>
-    <row r="77" ht="12.75">
+        <v>6.48</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B77" s="4">
-        <v>6.3600000000000003</v>
-      </c>
-    </row>
-    <row r="78" ht="12.75">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>40694</v>
       </c>
       <c r="B78" s="4">
-        <v>6.3300000000000001</v>
-      </c>
-    </row>
-    <row r="79" ht="12.75">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B79" s="4">
-        <v>6.3600000000000003</v>
-      </c>
-    </row>
-    <row r="80" ht="12.75">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>40755</v>
       </c>
       <c r="B80" s="4">
-        <v>6.3300000000000001</v>
-      </c>
-    </row>
-    <row r="81" ht="12.75">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>40786</v>
       </c>
       <c r="B81" s="4">
-        <v>6.5099999999999998</v>
-      </c>
-    </row>
-    <row r="82" ht="12.75">
+        <v>6.51</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B82" s="4">
-        <v>6.4199999999999999</v>
-      </c>
-    </row>
-    <row r="83" ht="12.75">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>40847</v>
       </c>
       <c r="B83" s="4">
-        <v>6.4199999999999999</v>
-      </c>
-    </row>
-    <row r="84" ht="12.75">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B84" s="4">
-        <v>6.5099999999999998</v>
-      </c>
-    </row>
-    <row r="85" ht="12.75">
+        <v>6.51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>40908</v>
       </c>
       <c r="B85" s="4">
-        <v>6.4800000000000004</v>
-      </c>
-    </row>
-    <row r="86" ht="12.75">
+        <v>6.48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>40939</v>
       </c>
       <c r="B86" s="4">
-        <v>6.3600000000000003</v>
-      </c>
-    </row>
-    <row r="87" ht="12.75">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>37</v>
       </c>
@@ -1605,39 +1343,39 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="88" ht="12.75">
+    <row r="88" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>40999</v>
       </c>
       <c r="B88" s="4">
-        <v>6.1500000000000004</v>
-      </c>
-    </row>
-    <row r="89" ht="12.75">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B89" s="4">
-        <v>6.3300000000000001</v>
-      </c>
-    </row>
-    <row r="90" ht="12.75">
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>41060</v>
       </c>
       <c r="B90" s="4">
-        <v>6.4199999999999999</v>
-      </c>
-    </row>
-    <row r="91" ht="12.75">
+        <v>6.42</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B91" s="4">
-        <v>6.2400000000000002</v>
-      </c>
-    </row>
-    <row r="92" ht="12.75">
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>41121</v>
       </c>
@@ -1645,7 +1383,7 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="93" ht="12.75">
+    <row r="93" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>41152</v>
       </c>
@@ -1653,39 +1391,39 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="94" ht="12.75">
+    <row r="94" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B94" s="4">
-        <v>6.0899999999999999</v>
-      </c>
-    </row>
-    <row r="95" ht="12.75">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>41213</v>
       </c>
       <c r="B95" s="4">
-        <v>6.0599999999999996</v>
-      </c>
-    </row>
-    <row r="96" ht="12.75">
+        <v>6.06</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B96" s="4">
-        <v>5.7599999999999998</v>
-      </c>
-    </row>
-    <row r="97" ht="12.75">
+        <v>5.76</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>41274</v>
       </c>
       <c r="B97" s="4">
-        <v>5.7300000000000004</v>
-      </c>
-    </row>
-    <row r="98" ht="12.75">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>41305</v>
       </c>
@@ -1693,119 +1431,119 @@
         <v>8.8800000000000008</v>
       </c>
     </row>
-    <row r="99" ht="12.75">
+    <row r="99" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B99" s="4">
-        <v>5.7000000000000002</v>
-      </c>
-    </row>
-    <row r="100" ht="12.75">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>41364</v>
       </c>
       <c r="B100" s="4">
-        <v>6.0599999999999996</v>
-      </c>
-    </row>
-    <row r="101" ht="12.75">
+        <v>6.06</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B101" s="4">
-        <v>5.8200000000000003</v>
-      </c>
-    </row>
-    <row r="102" ht="12.75">
+        <v>5.82</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>41425</v>
       </c>
       <c r="B102" s="4">
-        <v>5.7300000000000004</v>
-      </c>
-    </row>
-    <row r="103" ht="12.75">
+        <v>5.73</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B103" s="4">
-        <v>5.6399999999999997</v>
-      </c>
-    </row>
-    <row r="104" ht="12.75">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>41486</v>
       </c>
       <c r="B104" s="4">
-        <v>6.0599999999999996</v>
-      </c>
-    </row>
-    <row r="105" ht="12.75">
+        <v>6.06</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>41517</v>
       </c>
       <c r="B105" s="4">
-        <v>5.9100000000000001</v>
-      </c>
-    </row>
-    <row r="106" ht="12.75">
+        <v>5.91</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B106" s="4">
-        <v>6.2699999999999996</v>
-      </c>
-    </row>
-    <row r="107" ht="12.75">
+        <v>6.27</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>41578</v>
       </c>
       <c r="B107" s="4">
-        <v>6.1200000000000001</v>
-      </c>
-    </row>
-    <row r="108" ht="12.75">
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B108" s="4">
-        <v>6.1799999999999997</v>
-      </c>
-    </row>
-    <row r="109" ht="12.75">
+        <v>6.18</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>41639</v>
       </c>
       <c r="B109" s="4">
-        <v>5.8799999999999999</v>
-      </c>
-    </row>
-    <row r="110" ht="12.75">
+        <v>5.88</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>41670</v>
       </c>
       <c r="B110" s="4">
-        <v>6.0300000000000002</v>
-      </c>
-    </row>
-    <row r="111" ht="12.75">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B111" s="4">
-        <v>5.8200000000000003</v>
-      </c>
-    </row>
-    <row r="112" ht="12.75">
+        <v>5.82</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>41729</v>
       </c>
       <c r="B112" s="4">
-        <v>6.1500000000000004</v>
-      </c>
-    </row>
-    <row r="113" ht="12.75">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>48</v>
       </c>
@@ -1813,71 +1551,71 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="114" ht="12.75">
+    <row r="114" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>41790</v>
       </c>
       <c r="B114" s="4">
-        <v>6.3899999999999997</v>
-      </c>
-    </row>
-    <row r="115" ht="12.75">
+        <v>6.39</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B115" s="4">
-        <v>6.0300000000000002</v>
-      </c>
-    </row>
-    <row r="116" ht="12.75">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>41851</v>
       </c>
       <c r="B116" s="4">
-        <v>6.0300000000000002</v>
-      </c>
-    </row>
-    <row r="117" ht="12.75">
+        <v>6.03</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>41882</v>
       </c>
       <c r="B117" s="4">
-        <v>6.3600000000000003</v>
-      </c>
-    </row>
-    <row r="118" ht="12.75">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B118" s="4">
-        <v>6.1500000000000004</v>
-      </c>
-    </row>
-    <row r="119" ht="12.75">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>41943</v>
       </c>
       <c r="B119" s="4">
-        <v>6.3600000000000003</v>
-      </c>
-    </row>
-    <row r="120" ht="12.75">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B120" s="4">
-        <v>6.4500000000000002</v>
-      </c>
-    </row>
-    <row r="121" ht="12.75">
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>42004</v>
       </c>
       <c r="B121" s="4">
-        <v>6.3600000000000003</v>
-      </c>
-    </row>
-    <row r="122" ht="12.75">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>42035</v>
       </c>
@@ -1885,47 +1623,47 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="123" ht="12.75">
+    <row r="123" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B123" s="4">
-        <v>6.5999999999999996</v>
-      </c>
-    </row>
-    <row r="124" ht="12.75">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>42094</v>
       </c>
       <c r="B124" s="4">
-        <v>6.3600000000000003</v>
-      </c>
-    </row>
-    <row r="125" ht="12.75">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B125" s="4">
-        <v>6.2400000000000002</v>
-      </c>
-    </row>
-    <row r="126" ht="12.75">
+        <v>6.24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>42155</v>
       </c>
       <c r="B126" s="4">
-        <v>6.3899999999999997</v>
-      </c>
-    </row>
-    <row r="127" ht="12.75">
+        <v>6.39</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B127" s="4">
-        <v>6.1799999999999997</v>
-      </c>
-    </row>
-    <row r="128" ht="12.75">
+        <v>6.18</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
         <v>42216</v>
       </c>
@@ -1933,31 +1671,31 @@
         <v>5.46</v>
       </c>
     </row>
-    <row r="129" ht="12.75">
+    <row r="129" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
         <v>42247</v>
       </c>
       <c r="B129" s="4">
-        <v>5.4299999999999997</v>
-      </c>
-    </row>
-    <row r="130" ht="12.75">
+        <v>5.43</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B130" s="4">
-        <v>5.5199999999999996</v>
-      </c>
-    </row>
-    <row r="131" ht="12.75">
+        <v>5.52</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
         <v>42308</v>
       </c>
       <c r="B131" s="4">
-        <v>6.7199999999999998</v>
-      </c>
-    </row>
-    <row r="132" ht="12.75">
+        <v>6.72</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>56</v>
       </c>
@@ -1965,7 +1703,7 @@
         <v>8.1300000000000008</v>
       </c>
     </row>
-    <row r="133" ht="12.75">
+    <row r="133" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
         <v>42369</v>
       </c>
@@ -1973,23 +1711,23 @@
         <v>8.2200000000000006</v>
       </c>
     </row>
-    <row r="134" ht="12.75">
+    <row r="134" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
         <v>42400</v>
       </c>
       <c r="B134" s="4">
-        <v>8.5199999999999996</v>
-      </c>
-    </row>
-    <row r="135" ht="12.75">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B135" s="4">
-        <v>9.4199999999999999</v>
-      </c>
-    </row>
-    <row r="136" ht="12.75">
+        <v>9.42</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
         <v>42460</v>
       </c>
@@ -1997,15 +1735,15 @@
         <v>9.7200000000000006</v>
       </c>
     </row>
-    <row r="137" ht="12.75">
+    <row r="137" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B137" s="4">
-        <v>9.1799999999999997</v>
-      </c>
-    </row>
-    <row r="138" ht="12.75">
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
         <v>42521</v>
       </c>
@@ -2013,23 +1751,23 @@
         <v>9.1199999999999992</v>
       </c>
     </row>
-    <row r="139" ht="12.75">
+    <row r="139" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B139" s="4">
-        <v>9.1799999999999997</v>
-      </c>
-    </row>
-    <row r="140" ht="12.75">
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
         <v>42582</v>
       </c>
       <c r="B140" s="4">
-        <v>9.9900000000000002</v>
-      </c>
-    </row>
-    <row r="141" ht="12.75">
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
         <v>42613</v>
       </c>
@@ -2037,23 +1775,23 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="142" ht="12.75">
+    <row r="142" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B142" s="4">
-        <v>9.0600000000000005</v>
-      </c>
-    </row>
-    <row r="143" ht="12.75">
+        <v>9.06</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
         <v>42674</v>
       </c>
       <c r="B143" s="4">
-        <v>10.710000000000001</v>
-      </c>
-    </row>
-    <row r="144" ht="12.75">
+        <v>10.71</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>61</v>
       </c>
@@ -2061,7 +1799,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="145" ht="12.75">
+    <row r="145" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
         <v>42735</v>
       </c>
@@ -2069,7 +1807,7 @@
         <v>10.74</v>
       </c>
     </row>
-    <row r="146" ht="12.75">
+    <row r="146" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
         <v>42766</v>
       </c>
@@ -2077,7 +1815,7 @@
         <v>10.44</v>
       </c>
     </row>
-    <row r="147" ht="12.75">
+    <row r="147" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>62</v>
       </c>
@@ -2085,7 +1823,7 @@
         <v>10.050000000000001</v>
       </c>
     </row>
-    <row r="148" ht="12.75">
+    <row r="148" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
         <v>42825</v>
       </c>
@@ -2093,31 +1831,31 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" ht="12.75">
+    <row r="149" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B149" s="4">
-        <v>9.6600000000000001</v>
-      </c>
-    </row>
-    <row r="150" ht="12.75">
+        <v>9.66</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
         <v>42886</v>
       </c>
       <c r="B150" s="4">
-        <v>9.1500000000000004</v>
-      </c>
-    </row>
-    <row r="151" ht="12.75">
+        <v>9.15</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B151" s="4">
-        <v>8.7599999999999998</v>
-      </c>
-    </row>
-    <row r="152" ht="12.75">
+        <v>8.76</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="2">
         <v>42947</v>
       </c>
@@ -2125,23 +1863,23 @@
         <v>8.2200000000000006</v>
       </c>
     </row>
-    <row r="153" ht="12.75">
+    <row r="153" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A153" s="2">
         <v>42978</v>
       </c>
       <c r="B153" s="4">
-        <v>7.9800000000000004</v>
-      </c>
-    </row>
-    <row r="154" ht="12.75">
+        <v>7.98</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B154" s="4">
-        <v>7.1100000000000003</v>
-      </c>
-    </row>
-    <row r="155" ht="12.75">
+        <v>7.11</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="2">
         <v>43039</v>
       </c>
@@ -2149,31 +1887,31 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="156" ht="12.75">
+    <row r="156" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B156" s="4">
-        <v>6.7199999999999998</v>
-      </c>
-    </row>
-    <row r="157" ht="12.75">
+        <v>6.72</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="2">
         <v>43100</v>
       </c>
       <c r="B157" s="4">
-        <v>6.8099999999999996</v>
-      </c>
-    </row>
-    <row r="158" ht="12.75">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="2">
         <v>43131</v>
       </c>
       <c r="B158" s="4">
-        <v>6.9000000000000004</v>
-      </c>
-    </row>
-    <row r="159" ht="12.75">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>67</v>
       </c>
@@ -2181,47 +1919,47 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="160" ht="12.75">
+    <row r="160" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A160" s="2">
         <v>43190</v>
       </c>
       <c r="B160" s="4">
-        <v>6.7199999999999998</v>
-      </c>
-    </row>
-    <row r="161" ht="12.75">
+        <v>6.72</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B161" s="4">
-        <v>6.9000000000000004</v>
-      </c>
-    </row>
-    <row r="162" ht="12.75">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A162" s="2">
         <v>43251</v>
       </c>
       <c r="B162" s="4">
-        <v>6.4500000000000002</v>
-      </c>
-    </row>
-    <row r="163" ht="12.75">
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B163" s="4">
-        <v>6.9299999999999997</v>
-      </c>
-    </row>
-    <row r="164" ht="12.75">
+        <v>6.93</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A164" s="2">
         <v>43312</v>
       </c>
       <c r="B164" s="4">
-        <v>7.3499999999999996</v>
-      </c>
-    </row>
-    <row r="165" ht="12.75">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A165" s="2">
         <v>43343</v>
       </c>
@@ -2229,47 +1967,47 @@
         <v>7.29</v>
       </c>
     </row>
-    <row r="166" ht="12.75">
+    <row r="166" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B166" s="4">
-        <v>7.1699999999999999</v>
-      </c>
-    </row>
-    <row r="167" ht="12.75">
+        <v>7.17</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A167" s="2">
         <v>43404</v>
       </c>
       <c r="B167" s="4">
-        <v>7.0499999999999998</v>
-      </c>
-    </row>
-    <row r="168" ht="12.75">
+        <v>7.05</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B168" s="4">
-        <v>7.4100000000000001</v>
-      </c>
-    </row>
-    <row r="169" ht="12.75">
+        <v>7.41</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A169" s="2">
         <v>43465</v>
       </c>
       <c r="B169" s="4">
-        <v>7.8899999999999997</v>
-      </c>
-    </row>
-    <row r="170" ht="12.75">
+        <v>7.89</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A170" s="2">
         <v>43496</v>
       </c>
       <c r="B170" s="4">
-        <v>7.4699999999999998</v>
-      </c>
-    </row>
-    <row r="171" ht="12.75">
+        <v>7.47</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>72</v>
       </c>
@@ -2277,15 +2015,15 @@
         <v>7.71</v>
       </c>
     </row>
-    <row r="172" ht="12.75">
+    <row r="172" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A172" s="2">
         <v>43555</v>
       </c>
       <c r="B172" s="4">
-        <v>7.7400000000000002</v>
-      </c>
-    </row>
-    <row r="173" ht="12.75">
+        <v>7.74</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>73</v>
       </c>
@@ -2293,47 +2031,47 @@
         <v>8.1300000000000008</v>
       </c>
     </row>
-    <row r="174" ht="12.75">
+    <row r="174" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A174" s="2">
         <v>43616</v>
       </c>
       <c r="B174" s="4">
-        <v>7.6500000000000004</v>
-      </c>
-    </row>
-    <row r="175" ht="12.75">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B175" s="4">
-        <v>7.2599999999999998</v>
-      </c>
-    </row>
-    <row r="176" ht="12.75">
+        <v>7.26</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A176" s="2">
         <v>43677</v>
       </c>
       <c r="B176" s="4">
-        <v>7.1399999999999997</v>
-      </c>
-    </row>
-    <row r="177" ht="12.75">
+        <v>7.14</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A177" s="2">
         <v>43708</v>
       </c>
       <c r="B177" s="4">
-        <v>6.8099999999999996</v>
-      </c>
-    </row>
-    <row r="178" ht="12.75">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B178" s="4">
-        <v>7.1100000000000003</v>
-      </c>
-    </row>
-    <row r="179" ht="12.75">
+        <v>7.11</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
         <v>43769</v>
       </c>
@@ -2341,119 +2079,119 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="180" ht="12.75">
+    <row r="180" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B180" s="4">
-        <v>6.5999999999999996</v>
-      </c>
-    </row>
-    <row r="181" ht="12.75">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A181" s="2">
         <v>43830</v>
       </c>
       <c r="B181" s="4">
-        <v>6.8700000000000001</v>
-      </c>
-    </row>
-    <row r="182" ht="12.75">
+        <v>6.87</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A182" s="2">
         <v>43861</v>
       </c>
       <c r="B182" s="4">
-        <v>7.1699999999999999</v>
-      </c>
-    </row>
-    <row r="183" ht="12.75">
+        <v>7.17</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B183" s="4">
-        <v>7.3200000000000003</v>
-      </c>
-    </row>
-    <row r="184" ht="12.75">
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A184" s="2">
         <v>43921</v>
       </c>
       <c r="B184" s="4">
-        <v>7.3200000000000003</v>
-      </c>
-    </row>
-    <row r="185" ht="12.75">
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B185" s="4">
-        <v>7.9500000000000002</v>
-      </c>
-    </row>
-    <row r="186" ht="12.75">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A186" s="2">
         <v>43982</v>
       </c>
       <c r="B186" s="4">
-        <v>8.0700000000000003</v>
-      </c>
-    </row>
-    <row r="187" ht="12.75">
+        <v>8.07</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B187" s="4">
-        <v>8.0099999999999998</v>
-      </c>
-    </row>
-    <row r="188" ht="12.75">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A188" s="2">
         <v>44043</v>
       </c>
       <c r="B188" s="4">
-        <v>8.3399999999999999</v>
-      </c>
-    </row>
-    <row r="189" ht="12.75">
+        <v>8.34</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A189" s="2">
         <v>44074</v>
       </c>
       <c r="B189" s="4">
-        <v>7.8600000000000003</v>
-      </c>
-    </row>
-    <row r="190" ht="12.75">
+        <v>7.86</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B190" s="4">
-        <v>8.5199999999999996</v>
-      </c>
-    </row>
-    <row r="191" ht="12.75">
+        <v>8.52</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A191" s="2">
         <v>44135</v>
       </c>
       <c r="B191" s="4">
-        <v>9.1799999999999997</v>
-      </c>
-    </row>
-    <row r="192" ht="12.75">
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B192" s="4">
-        <v>8.9399999999999995</v>
-      </c>
-    </row>
-    <row r="193" ht="12.75">
+        <v>8.94</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A193" s="2">
         <v>44196</v>
       </c>
       <c r="B193" s="4">
-        <v>9.3300000000000001</v>
-      </c>
-    </row>
-    <row r="194" ht="12.75">
+        <v>9.33</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A194" s="2">
         <v>44227</v>
       </c>
@@ -2461,15 +2199,15 @@
         <v>8.4600000000000009</v>
       </c>
     </row>
-    <row r="195" ht="12.75">
+    <row r="195" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B195" s="4">
-        <v>8.8499999999999996</v>
-      </c>
-    </row>
-    <row r="196" ht="12.75">
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A196" s="2">
         <v>44286</v>
       </c>
@@ -2477,23 +2215,23 @@
         <v>9.5399999999999991</v>
       </c>
     </row>
-    <row r="197" ht="12.75">
+    <row r="197" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B197" s="4">
-        <v>9.8399999999999999</v>
-      </c>
-    </row>
-    <row r="198" ht="12.75">
+        <v>9.84</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A198" s="2">
         <v>44347</v>
       </c>
       <c r="B198" s="4">
-        <v>10.890000000000001</v>
-      </c>
-    </row>
-    <row r="199" ht="12.75">
+        <v>10.89</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
         <v>84</v>
       </c>
@@ -2501,7 +2239,7 @@
         <v>11.07</v>
       </c>
     </row>
-    <row r="200" ht="15.75" customHeight="1">
+    <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="2">
         <v>44408</v>
       </c>
@@ -2509,7 +2247,7 @@
         <v>11.43</v>
       </c>
     </row>
-    <row r="201" ht="15.75" customHeight="1">
+    <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>85</v>
       </c>
@@ -2518,15 +2256,15 @@
         <v>12.09</v>
       </c>
     </row>
-    <row r="202" ht="15.75" customHeight="1">
+    <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B202" s="4">
-        <v>12.720000000000001</v>
-      </c>
-    </row>
-    <row r="203" ht="15.75" customHeight="1">
+        <v>12.72</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
         <v>87</v>
       </c>
@@ -2534,15 +2272,15 @@
         <v>11.73</v>
       </c>
     </row>
-    <row r="204" ht="15.75" customHeight="1">
+    <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B204" s="4">
-        <v>12.119999999999999</v>
-      </c>
-    </row>
-    <row r="205" ht="15.75" customHeight="1">
+        <v>12.12</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="2">
         <v>44561</v>
       </c>
@@ -2550,7 +2288,7 @@
         <v>12.66</v>
       </c>
     </row>
-    <row r="206" ht="15.75" customHeight="1">
+    <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>44592</v>
       </c>
@@ -2558,23 +2296,23 @@
         <v>12.93</v>
       </c>
     </row>
-    <row r="207" ht="15.75" customHeight="1">
+    <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B207" s="4">
-        <v>13.289999999999999</v>
-      </c>
-    </row>
-    <row r="208" ht="15.75" customHeight="1">
+        <v>13.29</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>44651</v>
       </c>
       <c r="B208" s="4">
-        <v>12.779999999999999</v>
-      </c>
-    </row>
-    <row r="209" ht="15.75" customHeight="1">
+        <v>12.78</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
         <v>90</v>
       </c>
@@ -2582,23 +2320,23 @@
         <v>13.26</v>
       </c>
     </row>
-    <row r="210" ht="15.75" customHeight="1">
+    <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>44712</v>
       </c>
       <c r="B210" s="4">
-        <v>13.289999999999999</v>
-      </c>
-    </row>
-    <row r="211" ht="15.75" customHeight="1">
+        <v>13.29</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B211" s="4">
-        <v>13.199999999999999</v>
-      </c>
-    </row>
-    <row r="212" ht="15.75" customHeight="1">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>44773</v>
       </c>
@@ -2606,7 +2344,7 @@
         <v>13.17</v>
       </c>
     </row>
-    <row r="213" ht="15.75" customHeight="1">
+    <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>44804</v>
       </c>
@@ -2614,7 +2352,7 @@
         <v>13.08</v>
       </c>
     </row>
-    <row r="214" ht="15.75" customHeight="1">
+    <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
         <v>92</v>
       </c>
@@ -2622,31 +2360,31 @@
         <v>12.57</v>
       </c>
     </row>
-    <row r="215" ht="15.75" customHeight="1">
+    <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>44865</v>
       </c>
       <c r="B215" s="4">
-        <v>12.720000000000001</v>
-      </c>
-    </row>
-    <row r="216" ht="15.75" customHeight="1">
+        <v>12.72</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B216" s="4">
-        <v>12.779999999999999</v>
-      </c>
-    </row>
-    <row r="217" ht="15.75" customHeight="1">
+        <v>12.78</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>44926</v>
       </c>
       <c r="B217" s="4">
-        <v>13.380000000000001</v>
-      </c>
-    </row>
-    <row r="218" ht="15.75" customHeight="1">
+        <v>13.38</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>44957</v>
       </c>
@@ -2654,15 +2392,15 @@
         <v>12.84</v>
       </c>
     </row>
-    <row r="219" ht="15.75" customHeight="1">
+    <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B219" s="4">
-        <v>13.199999999999999</v>
-      </c>
-    </row>
-    <row r="220" ht="15.75" customHeight="1">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>45016</v>
       </c>
@@ -2670,15 +2408,15 @@
         <v>11.82</v>
       </c>
     </row>
-    <row r="221" ht="15.75" customHeight="1">
+    <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B221" s="4">
-        <v>11.970000000000001</v>
-      </c>
-    </row>
-    <row r="222" ht="15.75" customHeight="1">
+        <v>11.97</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>45077</v>
       </c>
@@ -2686,7 +2424,7 @@
         <v>13.74</v>
       </c>
     </row>
-    <row r="223" ht="15.75" customHeight="1">
+    <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="1" t="s">
         <v>96</v>
       </c>
@@ -2694,7 +2432,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="224" ht="15.75" customHeight="1">
+    <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>45138</v>
       </c>
@@ -2702,15 +2440,15 @@
         <v>13.77</v>
       </c>
     </row>
-    <row r="225" ht="15.75" customHeight="1">
+    <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>45169</v>
       </c>
       <c r="B225" s="4">
-        <v>13.529999999999999</v>
-      </c>
-    </row>
-    <row r="226" ht="15.75" customHeight="1">
+        <v>13.53</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>97</v>
       </c>
@@ -2718,7 +2456,7 @@
         <v>13.41</v>
       </c>
     </row>
-    <row r="227" ht="15.75" customHeight="1">
+    <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>45230</v>
       </c>
@@ -2726,7 +2464,7 @@
         <v>13.23</v>
       </c>
     </row>
-    <row r="228" ht="15.75" customHeight="1">
+    <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>98</v>
       </c>
@@ -2734,15 +2472,15 @@
         <v>13.59</v>
       </c>
     </row>
-    <row r="229" ht="15.75" customHeight="1">
+    <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>45291</v>
       </c>
       <c r="B229" s="4">
-        <v>14.039999999999999</v>
-      </c>
-    </row>
-    <row r="230" ht="15.75" customHeight="1">
+        <v>14.04</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>45322</v>
       </c>
@@ -2750,7 +2488,7 @@
         <v>13.92</v>
       </c>
     </row>
-    <row r="231" ht="15.75" customHeight="1">
+    <row r="231" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>99</v>
       </c>
@@ -2758,7 +2496,7 @@
         <v>14.43</v>
       </c>
     </row>
-    <row r="232" ht="15.75" customHeight="1">
+    <row r="232" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>45382</v>
       </c>
@@ -2766,7 +2504,7 @@
         <v>12.66</v>
       </c>
     </row>
-    <row r="233" ht="15.75" customHeight="1">
+    <row r="233" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>100</v>
       </c>
@@ -2774,15 +2512,15 @@
         <v>13.44</v>
       </c>
     </row>
-    <row r="234" ht="15.75" customHeight="1">
+    <row r="234" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>45443</v>
       </c>
       <c r="B234" s="4">
-        <v>13.140000000000001</v>
-      </c>
-    </row>
-    <row r="235" ht="15.75" customHeight="1">
+        <v>13.14</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>101</v>
       </c>
@@ -2790,7 +2528,7 @@
         <v>13.56</v>
       </c>
     </row>
-    <row r="236" ht="15.75" customHeight="1">
+    <row r="236" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>45504</v>
       </c>
@@ -2798,15 +2536,15 @@
         <v>12.81</v>
       </c>
     </row>
-    <row r="237" ht="15.75" customHeight="1">
+    <row r="237" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>45535</v>
       </c>
       <c r="B237" s="4">
-        <v>13.619999999999999</v>
-      </c>
-    </row>
-    <row r="238" ht="15.75" customHeight="1">
+        <v>13.62</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>102</v>
       </c>
@@ -2814,7 +2552,7 @@
         <v>14.01</v>
       </c>
     </row>
-    <row r="239" ht="15.75" customHeight="1">
+    <row r="239" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>45596</v>
       </c>
@@ -2822,7 +2560,7 @@
         <v>14.19</v>
       </c>
     </row>
-    <row r="240" ht="15.75" customHeight="1">
+    <row r="240" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>103</v>
       </c>
@@ -2830,7 +2568,7 @@
         <v>14.43</v>
       </c>
     </row>
-    <row r="241" ht="15.75" customHeight="1">
+    <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>45657</v>
       </c>
@@ -2838,7 +2576,7 @@
         <v>14.31</v>
       </c>
     </row>
-    <row r="242" ht="15.75" customHeight="1">
+    <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>45688</v>
       </c>
@@ -2846,15 +2584,15 @@
         <v>13.83</v>
       </c>
     </row>
-    <row r="243" ht="15.75" customHeight="1">
+    <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B243" s="4">
-        <v>14.279999999999999</v>
-      </c>
-    </row>
-    <row r="244" ht="15.75" customHeight="1">
+        <v>14.28</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>45747</v>
       </c>
@@ -2862,7 +2600,7 @@
         <v>13.83</v>
       </c>
     </row>
-    <row r="245" ht="15.75" customHeight="1">
+    <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>105</v>
       </c>
@@ -2870,7 +2608,7 @@
         <v>13.41</v>
       </c>
     </row>
-    <row r="246" ht="15.75" customHeight="1">
+    <row r="246" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>45808</v>
       </c>
@@ -2878,10 +2616,16 @@
         <v>14.01</v>
       </c>
     </row>
+    <row r="247" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A247" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B247" s="4">
+        <v>13.59</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000008" footer="0.31496062000000008"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add prev jav-mar 2026 feat: add prev 2026 fix: ajuste estrutura projeto doc: Melhorar doc README
</commit_message>
<xml_diff>
--- a/data/datasets_produtos/ilheus/acucar_ilheus.xlsx
+++ b/data/datasets_produtos/ilheus/acucar_ilheus.xlsx
@@ -1,36 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Meus Codes\previsao_cestas\data\datasets_produtos\ilheus\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC55BFC-70C3-4C12-A3B3-8857F3BF1C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="acucar_ilheus" sheetId="1" r:id="rId1"/>
+    <sheet name="acucar_ilheus" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
 </workbook>
 </file>
@@ -368,18 +348,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="10"/>
-      <color indexed="64"/>
+      <sz val="10.000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -393,28 +373,28 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,8 +412,291 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -636,27 +899,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <outlinePr applyStyles="0" summaryBelow="0" summaryRight="0" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="B253" sqref="B253"/>
+    <sheetView topLeftCell="A220" zoomScale="100" workbookViewId="0">
+      <selection activeCell="B253" activeCellId="0" sqref="B253"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="1"/>
+    <col min="1" max="1" style="1" width="14.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -664,7 +926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2">
         <v>38383</v>
       </c>
@@ -672,7 +934,7 @@
         <v>3.21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -680,15 +942,15 @@
         <v>3.21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2">
         <v>38442</v>
       </c>
       <c r="B4" s="4">
-        <v>3.39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.3900000000000001</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -696,63 +958,63 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="2">
         <v>38503</v>
       </c>
       <c r="B6" s="4">
-        <v>3.42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.4199999999999999</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="4">
-        <v>3.24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.2400000000000002</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="2">
         <v>38564</v>
       </c>
       <c r="B8" s="4">
-        <v>3.39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.3900000000000001</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>38595</v>
       </c>
       <c r="B9" s="4">
-        <v>3.24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.2400000000000002</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="4">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.2999999999999998</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="2">
         <v>38656</v>
       </c>
       <c r="B11" s="4">
-        <v>3.51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.5099999999999998</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="4">
-        <v>3.66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.6600000000000001</v>
+      </c>
+    </row>
+    <row r="13" ht="12.75">
       <c r="A13" s="2">
         <v>38717</v>
       </c>
@@ -760,15 +1022,15 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" ht="12.75">
       <c r="A14" s="2">
         <v>38748</v>
       </c>
       <c r="B14" s="4">
-        <v>4.38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4.3799999999999999</v>
+      </c>
+    </row>
+    <row r="15" ht="12.75">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -776,7 +1038,7 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" ht="12.75">
       <c r="A16" s="2">
         <v>38807</v>
       </c>
@@ -784,47 +1046,47 @@
         <v>5.04</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" ht="12.75">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="4">
-        <v>5.28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.2800000000000002</v>
+      </c>
+    </row>
+    <row r="18" ht="12.75">
       <c r="A18" s="2">
         <v>38868</v>
       </c>
       <c r="B18" s="4">
-        <v>5.34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.3399999999999999</v>
+      </c>
+    </row>
+    <row r="19" ht="12.75">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="4">
-        <v>5.34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.3399999999999999</v>
+      </c>
+    </row>
+    <row r="20" ht="12.75">
       <c r="A20" s="2">
         <v>38929</v>
       </c>
       <c r="B20" s="4">
-        <v>5.34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.3399999999999999</v>
+      </c>
+    </row>
+    <row r="21" ht="12.75">
       <c r="A21" s="2">
         <v>38960</v>
       </c>
       <c r="B21" s="4">
-        <v>5.31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.3099999999999996</v>
+      </c>
+    </row>
+    <row r="22" ht="12.75">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -832,7 +1094,7 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" ht="12.75">
       <c r="A23" s="2">
         <v>39021</v>
       </c>
@@ -840,15 +1102,15 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" ht="12.75">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="4">
-        <v>4.38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4.3799999999999999</v>
+      </c>
+    </row>
+    <row r="25" ht="12.75">
       <c r="A25" s="2">
         <v>39082</v>
       </c>
@@ -856,15 +1118,15 @@
         <v>4.2300000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" ht="12.75">
       <c r="A26" s="2">
         <v>39113</v>
       </c>
       <c r="B26" s="4">
-        <v>4.17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4.1699999999999999</v>
+      </c>
+    </row>
+    <row r="27" ht="12.75">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
@@ -872,31 +1134,31 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" ht="12.75">
       <c r="A28" s="2">
         <v>39172</v>
       </c>
       <c r="B28" s="4">
-        <v>4.17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4.1699999999999999</v>
+      </c>
+    </row>
+    <row r="29" ht="12.75">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="4">
-        <v>4.17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4.1699999999999999</v>
+      </c>
+    </row>
+    <row r="30" ht="12.75">
       <c r="A30" s="2">
         <v>39233</v>
       </c>
       <c r="B30" s="4">
-        <v>3.93</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.9300000000000002</v>
+      </c>
+    </row>
+    <row r="31" ht="12.75">
       <c r="A31" s="2" t="s">
         <v>14</v>
       </c>
@@ -904,31 +1166,31 @@
         <v>3.48</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" ht="12.75">
       <c r="A32" s="2">
         <v>39294</v>
       </c>
       <c r="B32" s="4">
-        <v>3.06</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.0600000000000001</v>
+      </c>
+    </row>
+    <row r="33" ht="12.75">
       <c r="A33" s="2">
         <v>39325</v>
       </c>
       <c r="B33" s="4">
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.1499999999999999</v>
+      </c>
+    </row>
+    <row r="34" ht="12.75">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="4">
-        <v>3.03</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.0299999999999998</v>
+      </c>
+    </row>
+    <row r="35" ht="12.75">
       <c r="A35" s="2">
         <v>39386</v>
       </c>
@@ -936,111 +1198,111 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" ht="12.75">
       <c r="A36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B36" s="4">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>2.8799999999999999</v>
+      </c>
+    </row>
+    <row r="37" ht="12.75">
       <c r="A37" s="2">
         <v>39447</v>
       </c>
       <c r="B37" s="4">
-        <v>2.94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>2.9399999999999999</v>
+      </c>
+    </row>
+    <row r="38" ht="12.75">
       <c r="A38" s="2">
         <v>39478</v>
       </c>
       <c r="B38" s="4">
-        <v>3.06</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.0600000000000001</v>
+      </c>
+    </row>
+    <row r="39" ht="12.75">
       <c r="A39" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B39" s="4">
-        <v>3.06</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.0600000000000001</v>
+      </c>
+    </row>
+    <row r="40" ht="12.75">
       <c r="A40" s="2">
         <v>39538</v>
       </c>
       <c r="B40" s="4">
-        <v>3.24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.2400000000000002</v>
+      </c>
+    </row>
+    <row r="41" ht="12.75">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B41" s="4">
-        <v>3.36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.3599999999999999</v>
+      </c>
+    </row>
+    <row r="42" ht="12.75">
       <c r="A42" s="2">
         <v>39599</v>
       </c>
       <c r="B42" s="4">
-        <v>3.36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.3599999999999999</v>
+      </c>
+    </row>
+    <row r="43" ht="12.75">
       <c r="A43" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="4">
-        <v>3.39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.3900000000000001</v>
+      </c>
+    </row>
+    <row r="44" ht="12.75">
       <c r="A44" s="2">
         <v>39660</v>
       </c>
       <c r="B44" s="4">
-        <v>3.15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.1499999999999999</v>
+      </c>
+    </row>
+    <row r="45" ht="12.75">
       <c r="A45" s="2">
         <v>39691</v>
       </c>
       <c r="B45" s="4">
-        <v>3.24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.2400000000000002</v>
+      </c>
+    </row>
+    <row r="46" ht="12.75">
       <c r="A46" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B46" s="4">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.2999999999999998</v>
+      </c>
+    </row>
+    <row r="47" ht="12.75">
       <c r="A47" s="2">
         <v>39752</v>
       </c>
       <c r="B47" s="4">
-        <v>3.39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.3900000000000001</v>
+      </c>
+    </row>
+    <row r="48" ht="12.75">
       <c r="A48" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B48" s="4">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3.6000000000000001</v>
+      </c>
+    </row>
+    <row r="49" ht="12.75">
       <c r="A49" s="2">
         <v>39813</v>
       </c>
@@ -1048,7 +1310,7 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" ht="12.75">
       <c r="A50" s="2">
         <v>39844</v>
       </c>
@@ -1056,31 +1318,31 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" ht="12.75">
       <c r="A51" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B51" s="4">
-        <v>4.68</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4.6799999999999997</v>
+      </c>
+    </row>
+    <row r="52" ht="12.75">
       <c r="A52" s="2">
         <v>39903</v>
       </c>
       <c r="B52" s="4">
-        <v>4.92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4.9199999999999999</v>
+      </c>
+    </row>
+    <row r="53" ht="12.75">
       <c r="A53" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B53" s="4">
-        <v>5.01</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.0099999999999998</v>
+      </c>
+    </row>
+    <row r="54" ht="12.75">
       <c r="A54" s="2">
         <v>39964</v>
       </c>
@@ -1088,7 +1350,7 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" ht="12.75">
       <c r="A55" s="2" t="s">
         <v>24</v>
       </c>
@@ -1096,15 +1358,15 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" ht="12.75">
       <c r="A56" s="2">
         <v>40025</v>
       </c>
       <c r="B56" s="4">
-        <v>4.74</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4.7400000000000002</v>
+      </c>
+    </row>
+    <row r="57" ht="12.75">
       <c r="A57" s="2">
         <v>40056</v>
       </c>
@@ -1112,15 +1374,15 @@
         <v>4.71</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" ht="12.75">
       <c r="A58" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B58" s="4">
-        <v>5.22</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.2199999999999998</v>
+      </c>
+    </row>
+    <row r="59" ht="12.75">
       <c r="A59" s="2">
         <v>40117</v>
       </c>
@@ -1128,15 +1390,15 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" ht="12.75">
       <c r="A60" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B60" s="4">
-        <v>5.22</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.2199999999999998</v>
+      </c>
+    </row>
+    <row r="61" ht="12.75">
       <c r="A61" s="2">
         <v>40178</v>
       </c>
@@ -1144,207 +1406,207 @@
         <v>4.9800000000000004</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" ht="12.75">
       <c r="A62" s="2">
         <v>40209</v>
       </c>
       <c r="B62" s="4">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.5999999999999996</v>
+      </c>
+    </row>
+    <row r="63" ht="12.75">
       <c r="A63" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B63" s="4">
-        <v>6.78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.7800000000000002</v>
+      </c>
+    </row>
+    <row r="64" ht="12.75">
       <c r="A64" s="2">
         <v>40268</v>
       </c>
       <c r="B64" s="4">
-        <v>6.84</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.8399999999999999</v>
+      </c>
+    </row>
+    <row r="65" ht="12.75">
       <c r="A65" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B65" s="4">
-        <v>6.39</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3899999999999997</v>
+      </c>
+    </row>
+    <row r="66" ht="12.75">
       <c r="A66" s="2">
         <v>40329</v>
       </c>
       <c r="B66" s="4">
-        <v>6.24</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.2400000000000002</v>
+      </c>
+    </row>
+    <row r="67" ht="12.75">
       <c r="A67" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B67" s="4">
-        <v>5.73</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.7300000000000004</v>
+      </c>
+    </row>
+    <row r="68" ht="12.75">
       <c r="A68" s="2">
         <v>40390</v>
       </c>
       <c r="B68" s="4">
-        <v>5.01</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.0099999999999998</v>
+      </c>
+    </row>
+    <row r="69" ht="12.75">
       <c r="A69" s="2">
         <v>40421</v>
       </c>
       <c r="B69" s="4">
-        <v>4.83</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>4.8300000000000001</v>
+      </c>
+    </row>
+    <row r="70" ht="12.75">
       <c r="A70" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B70" s="4">
-        <v>5.31</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.3099999999999996</v>
+      </c>
+    </row>
+    <row r="71" ht="12.75">
       <c r="A71" s="2">
         <v>40482</v>
       </c>
       <c r="B71" s="4">
-        <v>6.03</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.0300000000000002</v>
+      </c>
+    </row>
+    <row r="72" ht="12.75">
       <c r="A72" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B72" s="4">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.5999999999999996</v>
+      </c>
+    </row>
+    <row r="73" ht="12.75">
       <c r="A73" s="2">
         <v>40543</v>
       </c>
       <c r="B73" s="4">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.2999999999999998</v>
+      </c>
+    </row>
+    <row r="74" ht="12.75">
       <c r="A74" s="2">
         <v>40574</v>
       </c>
       <c r="B74" s="4">
-        <v>6.39</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3899999999999997</v>
+      </c>
+    </row>
+    <row r="75" ht="12.75">
       <c r="A75" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B75" s="4">
-        <v>6.45</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.4500000000000002</v>
+      </c>
+    </row>
+    <row r="76" ht="12.75">
       <c r="A76" s="2">
         <v>40633</v>
       </c>
       <c r="B76" s="4">
-        <v>6.48</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.4800000000000004</v>
+      </c>
+    </row>
+    <row r="77" ht="12.75">
       <c r="A77" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B77" s="4">
-        <v>6.36</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3600000000000003</v>
+      </c>
+    </row>
+    <row r="78" ht="12.75">
       <c r="A78" s="2">
         <v>40694</v>
       </c>
       <c r="B78" s="4">
-        <v>6.33</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3300000000000001</v>
+      </c>
+    </row>
+    <row r="79" ht="12.75">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B79" s="4">
-        <v>6.36</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3600000000000003</v>
+      </c>
+    </row>
+    <row r="80" ht="12.75">
       <c r="A80" s="2">
         <v>40755</v>
       </c>
       <c r="B80" s="4">
-        <v>6.33</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3300000000000001</v>
+      </c>
+    </row>
+    <row r="81" ht="12.75">
       <c r="A81" s="2">
         <v>40786</v>
       </c>
       <c r="B81" s="4">
-        <v>6.51</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.5099999999999998</v>
+      </c>
+    </row>
+    <row r="82" ht="12.75">
       <c r="A82" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B82" s="4">
-        <v>6.42</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.4199999999999999</v>
+      </c>
+    </row>
+    <row r="83" ht="12.75">
       <c r="A83" s="2">
         <v>40847</v>
       </c>
       <c r="B83" s="4">
-        <v>6.42</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.4199999999999999</v>
+      </c>
+    </row>
+    <row r="84" ht="12.75">
       <c r="A84" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B84" s="4">
-        <v>6.51</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.5099999999999998</v>
+      </c>
+    </row>
+    <row r="85" ht="12.75">
       <c r="A85" s="2">
         <v>40908</v>
       </c>
       <c r="B85" s="4">
-        <v>6.48</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.4800000000000004</v>
+      </c>
+    </row>
+    <row r="86" ht="12.75">
       <c r="A86" s="2">
         <v>40939</v>
       </c>
       <c r="B86" s="4">
-        <v>6.36</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3600000000000003</v>
+      </c>
+    </row>
+    <row r="87" ht="12.75">
       <c r="A87" s="2" t="s">
         <v>37</v>
       </c>
@@ -1352,39 +1614,39 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" ht="12.75">
       <c r="A88" s="2">
         <v>40999</v>
       </c>
       <c r="B88" s="4">
-        <v>6.15</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.1500000000000004</v>
+      </c>
+    </row>
+    <row r="89" ht="12.75">
       <c r="A89" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B89" s="4">
-        <v>6.33</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3300000000000001</v>
+      </c>
+    </row>
+    <row r="90" ht="12.75">
       <c r="A90" s="2">
         <v>41060</v>
       </c>
       <c r="B90" s="4">
-        <v>6.42</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.4199999999999999</v>
+      </c>
+    </row>
+    <row r="91" ht="12.75">
       <c r="A91" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B91" s="4">
-        <v>6.24</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.2400000000000002</v>
+      </c>
+    </row>
+    <row r="92" ht="12.75">
       <c r="A92" s="2">
         <v>41121</v>
       </c>
@@ -1392,7 +1654,7 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" ht="12.75">
       <c r="A93" s="2">
         <v>41152</v>
       </c>
@@ -1400,39 +1662,39 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" ht="12.75">
       <c r="A94" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B94" s="4">
-        <v>6.09</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.0899999999999999</v>
+      </c>
+    </row>
+    <row r="95" ht="12.75">
       <c r="A95" s="2">
         <v>41213</v>
       </c>
       <c r="B95" s="4">
-        <v>6.06</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.0599999999999996</v>
+      </c>
+    </row>
+    <row r="96" ht="12.75">
       <c r="A96" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B96" s="4">
-        <v>5.76</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.7599999999999998</v>
+      </c>
+    </row>
+    <row r="97" ht="12.75">
       <c r="A97" s="2">
         <v>41274</v>
       </c>
       <c r="B97" s="4">
-        <v>5.73</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.7300000000000004</v>
+      </c>
+    </row>
+    <row r="98" ht="12.75">
       <c r="A98" s="2">
         <v>41305</v>
       </c>
@@ -1440,119 +1702,119 @@
         <v>8.8800000000000008</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" ht="12.75">
       <c r="A99" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B99" s="4">
-        <v>5.7</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.7000000000000002</v>
+      </c>
+    </row>
+    <row r="100" ht="12.75">
       <c r="A100" s="2">
         <v>41364</v>
       </c>
       <c r="B100" s="4">
-        <v>6.06</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.0599999999999996</v>
+      </c>
+    </row>
+    <row r="101" ht="12.75">
       <c r="A101" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B101" s="4">
-        <v>5.82</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.8200000000000003</v>
+      </c>
+    </row>
+    <row r="102" ht="12.75">
       <c r="A102" s="2">
         <v>41425</v>
       </c>
       <c r="B102" s="4">
-        <v>5.73</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.7300000000000004</v>
+      </c>
+    </row>
+    <row r="103" ht="12.75">
       <c r="A103" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B103" s="4">
-        <v>5.64</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.6399999999999997</v>
+      </c>
+    </row>
+    <row r="104" ht="12.75">
       <c r="A104" s="2">
         <v>41486</v>
       </c>
       <c r="B104" s="4">
-        <v>6.06</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.0599999999999996</v>
+      </c>
+    </row>
+    <row r="105" ht="12.75">
       <c r="A105" s="2">
         <v>41517</v>
       </c>
       <c r="B105" s="4">
-        <v>5.91</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.9100000000000001</v>
+      </c>
+    </row>
+    <row r="106" ht="12.75">
       <c r="A106" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B106" s="4">
-        <v>6.27</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.2699999999999996</v>
+      </c>
+    </row>
+    <row r="107" ht="12.75">
       <c r="A107" s="2">
         <v>41578</v>
       </c>
       <c r="B107" s="4">
-        <v>6.12</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.1200000000000001</v>
+      </c>
+    </row>
+    <row r="108" ht="12.75">
       <c r="A108" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B108" s="4">
-        <v>6.18</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.1799999999999997</v>
+      </c>
+    </row>
+    <row r="109" ht="12.75">
       <c r="A109" s="2">
         <v>41639</v>
       </c>
       <c r="B109" s="4">
-        <v>5.88</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.8799999999999999</v>
+      </c>
+    </row>
+    <row r="110" ht="12.75">
       <c r="A110" s="2">
         <v>41670</v>
       </c>
       <c r="B110" s="4">
-        <v>6.03</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.0300000000000002</v>
+      </c>
+    </row>
+    <row r="111" ht="12.75">
       <c r="A111" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B111" s="4">
-        <v>5.82</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.8200000000000003</v>
+      </c>
+    </row>
+    <row r="112" ht="12.75">
       <c r="A112" s="2">
         <v>41729</v>
       </c>
       <c r="B112" s="4">
-        <v>6.15</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.1500000000000004</v>
+      </c>
+    </row>
+    <row r="113" ht="12.75">
       <c r="A113" s="2" t="s">
         <v>48</v>
       </c>
@@ -1560,71 +1822,71 @@
         <v>6.21</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" ht="12.75">
       <c r="A114" s="2">
         <v>41790</v>
       </c>
       <c r="B114" s="4">
-        <v>6.39</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3899999999999997</v>
+      </c>
+    </row>
+    <row r="115" ht="12.75">
       <c r="A115" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B115" s="4">
-        <v>6.03</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.0300000000000002</v>
+      </c>
+    </row>
+    <row r="116" ht="12.75">
       <c r="A116" s="2">
         <v>41851</v>
       </c>
       <c r="B116" s="4">
-        <v>6.03</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.0300000000000002</v>
+      </c>
+    </row>
+    <row r="117" ht="12.75">
       <c r="A117" s="2">
         <v>41882</v>
       </c>
       <c r="B117" s="4">
-        <v>6.36</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3600000000000003</v>
+      </c>
+    </row>
+    <row r="118" ht="12.75">
       <c r="A118" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B118" s="4">
-        <v>6.15</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.1500000000000004</v>
+      </c>
+    </row>
+    <row r="119" ht="12.75">
       <c r="A119" s="2">
         <v>41943</v>
       </c>
       <c r="B119" s="4">
-        <v>6.36</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3600000000000003</v>
+      </c>
+    </row>
+    <row r="120" ht="12.75">
       <c r="A120" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B120" s="4">
-        <v>6.45</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.4500000000000002</v>
+      </c>
+    </row>
+    <row r="121" ht="12.75">
       <c r="A121" s="2">
         <v>42004</v>
       </c>
       <c r="B121" s="4">
-        <v>6.36</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3600000000000003</v>
+      </c>
+    </row>
+    <row r="122" ht="12.75">
       <c r="A122" s="2">
         <v>42035</v>
       </c>
@@ -1632,47 +1894,47 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" ht="12.75">
       <c r="A123" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B123" s="4">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.5999999999999996</v>
+      </c>
+    </row>
+    <row r="124" ht="12.75">
       <c r="A124" s="2">
         <v>42094</v>
       </c>
       <c r="B124" s="4">
-        <v>6.36</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3600000000000003</v>
+      </c>
+    </row>
+    <row r="125" ht="12.75">
       <c r="A125" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B125" s="4">
-        <v>6.24</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.2400000000000002</v>
+      </c>
+    </row>
+    <row r="126" ht="12.75">
       <c r="A126" s="2">
         <v>42155</v>
       </c>
       <c r="B126" s="4">
-        <v>6.39</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.3899999999999997</v>
+      </c>
+    </row>
+    <row r="127" ht="12.75">
       <c r="A127" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B127" s="4">
-        <v>6.18</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.1799999999999997</v>
+      </c>
+    </row>
+    <row r="128" ht="12.75">
       <c r="A128" s="2">
         <v>42216</v>
       </c>
@@ -1680,31 +1942,31 @@
         <v>5.46</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" ht="12.75">
       <c r="A129" s="2">
         <v>42247</v>
       </c>
       <c r="B129" s="4">
-        <v>5.43</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.4299999999999997</v>
+      </c>
+    </row>
+    <row r="130" ht="12.75">
       <c r="A130" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B130" s="4">
-        <v>5.52</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5.5199999999999996</v>
+      </c>
+    </row>
+    <row r="131" ht="12.75">
       <c r="A131" s="2">
         <v>42308</v>
       </c>
       <c r="B131" s="4">
-        <v>6.72</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.7199999999999998</v>
+      </c>
+    </row>
+    <row r="132" ht="12.75">
       <c r="A132" s="2" t="s">
         <v>56</v>
       </c>
@@ -1712,7 +1974,7 @@
         <v>8.1300000000000008</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" ht="12.75">
       <c r="A133" s="2">
         <v>42369</v>
       </c>
@@ -1720,23 +1982,23 @@
         <v>8.2200000000000006</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" ht="12.75">
       <c r="A134" s="2">
         <v>42400</v>
       </c>
       <c r="B134" s="4">
-        <v>8.52</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8.5199999999999996</v>
+      </c>
+    </row>
+    <row r="135" ht="12.75">
       <c r="A135" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B135" s="4">
-        <v>9.42</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9.4199999999999999</v>
+      </c>
+    </row>
+    <row r="136" ht="12.75">
       <c r="A136" s="2">
         <v>42460</v>
       </c>
@@ -1744,15 +2006,15 @@
         <v>9.7200000000000006</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" ht="12.75">
       <c r="A137" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B137" s="4">
-        <v>9.18</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9.1799999999999997</v>
+      </c>
+    </row>
+    <row r="138" ht="12.75">
       <c r="A138" s="2">
         <v>42521</v>
       </c>
@@ -1760,23 +2022,23 @@
         <v>9.1199999999999992</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" ht="12.75">
       <c r="A139" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B139" s="4">
-        <v>9.18</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9.1799999999999997</v>
+      </c>
+    </row>
+    <row r="140" ht="12.75">
       <c r="A140" s="2">
         <v>42582</v>
       </c>
       <c r="B140" s="4">
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9.9900000000000002</v>
+      </c>
+    </row>
+    <row r="141" ht="12.75">
       <c r="A141" s="2">
         <v>42613</v>
       </c>
@@ -1784,23 +2046,23 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" ht="12.75">
       <c r="A142" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B142" s="4">
-        <v>9.06</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9.0600000000000005</v>
+      </c>
+    </row>
+    <row r="143" ht="12.75">
       <c r="A143" s="2">
         <v>42674</v>
       </c>
       <c r="B143" s="4">
-        <v>10.71</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>10.710000000000001</v>
+      </c>
+    </row>
+    <row r="144" ht="12.75">
       <c r="A144" s="2" t="s">
         <v>61</v>
       </c>
@@ -1808,7 +2070,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" ht="12.75">
       <c r="A145" s="2">
         <v>42735</v>
       </c>
@@ -1816,7 +2078,7 @@
         <v>10.74</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" ht="12.75">
       <c r="A146" s="2">
         <v>42766</v>
       </c>
@@ -1824,7 +2086,7 @@
         <v>10.44</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" ht="12.75">
       <c r="A147" s="2" t="s">
         <v>62</v>
       </c>
@@ -1832,7 +2094,7 @@
         <v>10.050000000000001</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" ht="12.75">
       <c r="A148" s="2">
         <v>42825</v>
       </c>
@@ -1840,31 +2102,31 @@
         <v>9</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" ht="12.75">
       <c r="A149" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B149" s="4">
-        <v>9.66</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9.6600000000000001</v>
+      </c>
+    </row>
+    <row r="150" ht="12.75">
       <c r="A150" s="2">
         <v>42886</v>
       </c>
       <c r="B150" s="4">
-        <v>9.15</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9.1500000000000004</v>
+      </c>
+    </row>
+    <row r="151" ht="12.75">
       <c r="A151" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B151" s="4">
-        <v>8.76</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8.7599999999999998</v>
+      </c>
+    </row>
+    <row r="152" ht="12.75">
       <c r="A152" s="2">
         <v>42947</v>
       </c>
@@ -1872,23 +2134,23 @@
         <v>8.2200000000000006</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" ht="12.75">
       <c r="A153" s="2">
         <v>42978</v>
       </c>
       <c r="B153" s="4">
-        <v>7.98</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.9800000000000004</v>
+      </c>
+    </row>
+    <row r="154" ht="12.75">
       <c r="A154" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B154" s="4">
-        <v>7.11</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.1100000000000003</v>
+      </c>
+    </row>
+    <row r="155" ht="12.75">
       <c r="A155" s="2">
         <v>43039</v>
       </c>
@@ -1896,31 +2158,31 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" ht="12.75">
       <c r="A156" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B156" s="4">
-        <v>6.72</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.7199999999999998</v>
+      </c>
+    </row>
+    <row r="157" ht="12.75">
       <c r="A157" s="2">
         <v>43100</v>
       </c>
       <c r="B157" s="4">
-        <v>6.81</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.8099999999999996</v>
+      </c>
+    </row>
+    <row r="158" ht="12.75">
       <c r="A158" s="2">
         <v>43131</v>
       </c>
       <c r="B158" s="4">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.9000000000000004</v>
+      </c>
+    </row>
+    <row r="159" ht="12.75">
       <c r="A159" s="2" t="s">
         <v>67</v>
       </c>
@@ -1928,47 +2190,47 @@
         <v>6.75</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" ht="12.75">
       <c r="A160" s="2">
         <v>43190</v>
       </c>
       <c r="B160" s="4">
-        <v>6.72</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.7199999999999998</v>
+      </c>
+    </row>
+    <row r="161" ht="12.75">
       <c r="A161" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B161" s="4">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.9000000000000004</v>
+      </c>
+    </row>
+    <row r="162" ht="12.75">
       <c r="A162" s="2">
         <v>43251</v>
       </c>
       <c r="B162" s="4">
-        <v>6.45</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.4500000000000002</v>
+      </c>
+    </row>
+    <row r="163" ht="12.75">
       <c r="A163" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B163" s="4">
-        <v>6.93</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.9299999999999997</v>
+      </c>
+    </row>
+    <row r="164" ht="12.75">
       <c r="A164" s="2">
         <v>43312</v>
       </c>
       <c r="B164" s="4">
-        <v>7.35</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.3499999999999996</v>
+      </c>
+    </row>
+    <row r="165" ht="12.75">
       <c r="A165" s="2">
         <v>43343</v>
       </c>
@@ -1976,47 +2238,47 @@
         <v>7.29</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" ht="12.75">
       <c r="A166" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B166" s="4">
-        <v>7.17</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.1699999999999999</v>
+      </c>
+    </row>
+    <row r="167" ht="12.75">
       <c r="A167" s="2">
         <v>43404</v>
       </c>
       <c r="B167" s="4">
-        <v>7.05</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.0499999999999998</v>
+      </c>
+    </row>
+    <row r="168" ht="12.75">
       <c r="A168" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B168" s="4">
-        <v>7.41</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.4100000000000001</v>
+      </c>
+    </row>
+    <row r="169" ht="12.75">
       <c r="A169" s="2">
         <v>43465</v>
       </c>
       <c r="B169" s="4">
-        <v>7.89</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.8899999999999997</v>
+      </c>
+    </row>
+    <row r="170" ht="12.75">
       <c r="A170" s="2">
         <v>43496</v>
       </c>
       <c r="B170" s="4">
-        <v>7.47</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.4699999999999998</v>
+      </c>
+    </row>
+    <row r="171" ht="12.75">
       <c r="A171" s="2" t="s">
         <v>72</v>
       </c>
@@ -2024,15 +2286,15 @@
         <v>7.71</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" ht="12.75">
       <c r="A172" s="2">
         <v>43555</v>
       </c>
       <c r="B172" s="4">
-        <v>7.74</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.7400000000000002</v>
+      </c>
+    </row>
+    <row r="173" ht="12.75">
       <c r="A173" s="2" t="s">
         <v>73</v>
       </c>
@@ -2040,47 +2302,47 @@
         <v>8.1300000000000008</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" ht="12.75">
       <c r="A174" s="2">
         <v>43616</v>
       </c>
       <c r="B174" s="4">
-        <v>7.65</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.6500000000000004</v>
+      </c>
+    </row>
+    <row r="175" ht="12.75">
       <c r="A175" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B175" s="4">
-        <v>7.26</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.2599999999999998</v>
+      </c>
+    </row>
+    <row r="176" ht="12.75">
       <c r="A176" s="2">
         <v>43677</v>
       </c>
       <c r="B176" s="4">
-        <v>7.14</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.1399999999999997</v>
+      </c>
+    </row>
+    <row r="177" ht="12.75">
       <c r="A177" s="2">
         <v>43708</v>
       </c>
       <c r="B177" s="4">
-        <v>6.81</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.8099999999999996</v>
+      </c>
+    </row>
+    <row r="178" ht="12.75">
       <c r="A178" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B178" s="4">
-        <v>7.11</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.1100000000000003</v>
+      </c>
+    </row>
+    <row r="179" ht="12.75">
       <c r="A179" s="2">
         <v>43769</v>
       </c>
@@ -2088,119 +2350,119 @@
         <v>6.54</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" ht="12.75">
       <c r="A180" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B180" s="4">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.5999999999999996</v>
+      </c>
+    </row>
+    <row r="181" ht="12.75">
       <c r="A181" s="2">
         <v>43830</v>
       </c>
       <c r="B181" s="4">
-        <v>6.87</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6.8700000000000001</v>
+      </c>
+    </row>
+    <row r="182" ht="12.75">
       <c r="A182" s="2">
         <v>43861</v>
       </c>
       <c r="B182" s="4">
-        <v>7.17</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.1699999999999999</v>
+      </c>
+    </row>
+    <row r="183" ht="12.75">
       <c r="A183" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B183" s="4">
-        <v>7.32</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.3200000000000003</v>
+      </c>
+    </row>
+    <row r="184" ht="12.75">
       <c r="A184" s="2">
         <v>43921</v>
       </c>
       <c r="B184" s="4">
-        <v>7.32</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.3200000000000003</v>
+      </c>
+    </row>
+    <row r="185" ht="12.75">
       <c r="A185" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B185" s="4">
-        <v>7.95</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.9500000000000002</v>
+      </c>
+    </row>
+    <row r="186" ht="12.75">
       <c r="A186" s="2">
         <v>43982</v>
       </c>
       <c r="B186" s="4">
-        <v>8.07</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8.0700000000000003</v>
+      </c>
+    </row>
+    <row r="187" ht="12.75">
       <c r="A187" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B187" s="4">
-        <v>8.01</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8.0099999999999998</v>
+      </c>
+    </row>
+    <row r="188" ht="12.75">
       <c r="A188" s="2">
         <v>44043</v>
       </c>
       <c r="B188" s="4">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8.3399999999999999</v>
+      </c>
+    </row>
+    <row r="189" ht="12.75">
       <c r="A189" s="2">
         <v>44074</v>
       </c>
       <c r="B189" s="4">
-        <v>7.86</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>7.8600000000000003</v>
+      </c>
+    </row>
+    <row r="190" ht="12.75">
       <c r="A190" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B190" s="4">
-        <v>8.52</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8.5199999999999996</v>
+      </c>
+    </row>
+    <row r="191" ht="12.75">
       <c r="A191" s="2">
         <v>44135</v>
       </c>
       <c r="B191" s="4">
-        <v>9.18</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9.1799999999999997</v>
+      </c>
+    </row>
+    <row r="192" ht="12.75">
       <c r="A192" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B192" s="4">
-        <v>8.94</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8.9399999999999995</v>
+      </c>
+    </row>
+    <row r="193" ht="12.75">
       <c r="A193" s="2">
         <v>44196</v>
       </c>
       <c r="B193" s="4">
-        <v>9.33</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9.3300000000000001</v>
+      </c>
+    </row>
+    <row r="194" ht="12.75">
       <c r="A194" s="2">
         <v>44227</v>
       </c>
@@ -2208,15 +2470,15 @@
         <v>8.4600000000000009</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" ht="12.75">
       <c r="A195" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B195" s="4">
-        <v>8.85</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8.8499999999999996</v>
+      </c>
+    </row>
+    <row r="196" ht="12.75">
       <c r="A196" s="2">
         <v>44286</v>
       </c>
@@ -2224,23 +2486,23 @@
         <v>9.5399999999999991</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" ht="12.75">
       <c r="A197" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B197" s="4">
-        <v>9.84</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>9.8399999999999999</v>
+      </c>
+    </row>
+    <row r="198" ht="12.75">
       <c r="A198" s="2">
         <v>44347</v>
       </c>
       <c r="B198" s="4">
-        <v>10.89</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+        <v>10.890000000000001</v>
+      </c>
+    </row>
+    <row r="199" ht="12.75">
       <c r="A199" s="2" t="s">
         <v>84</v>
       </c>
@@ -2248,7 +2510,7 @@
         <v>11.07</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" ht="15.75" customHeight="1">
       <c r="A200" s="2">
         <v>44408</v>
       </c>
@@ -2256,7 +2518,7 @@
         <v>11.43</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" ht="15.75" customHeight="1">
       <c r="A201" s="1" t="s">
         <v>85</v>
       </c>
@@ -2265,15 +2527,15 @@
         <v>12.09</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" ht="15.75" customHeight="1">
       <c r="A202" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B202" s="4">
-        <v>12.72</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12.720000000000001</v>
+      </c>
+    </row>
+    <row r="203" ht="15.75" customHeight="1">
       <c r="A203" s="1" t="s">
         <v>87</v>
       </c>
@@ -2281,15 +2543,15 @@
         <v>11.73</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" ht="15.75" customHeight="1">
       <c r="A204" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B204" s="4">
-        <v>12.12</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12.119999999999999</v>
+      </c>
+    </row>
+    <row r="205" ht="15.75" customHeight="1">
       <c r="A205" s="2">
         <v>44561</v>
       </c>
@@ -2297,7 +2559,7 @@
         <v>12.66</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" ht="15.75" customHeight="1">
       <c r="A206" s="1">
         <v>44592</v>
       </c>
@@ -2305,23 +2567,23 @@
         <v>12.93</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" ht="15.75" customHeight="1">
       <c r="A207" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B207" s="4">
-        <v>13.29</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13.289999999999999</v>
+      </c>
+    </row>
+    <row r="208" ht="15.75" customHeight="1">
       <c r="A208" s="1">
         <v>44651</v>
       </c>
       <c r="B208" s="4">
-        <v>12.78</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12.779999999999999</v>
+      </c>
+    </row>
+    <row r="209" ht="15.75" customHeight="1">
       <c r="A209" s="1" t="s">
         <v>90</v>
       </c>
@@ -2329,23 +2591,23 @@
         <v>13.26</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" ht="15.75" customHeight="1">
       <c r="A210" s="1">
         <v>44712</v>
       </c>
       <c r="B210" s="4">
-        <v>13.29</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13.289999999999999</v>
+      </c>
+    </row>
+    <row r="211" ht="15.75" customHeight="1">
       <c r="A211" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B211" s="4">
-        <v>13.2</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13.199999999999999</v>
+      </c>
+    </row>
+    <row r="212" ht="15.75" customHeight="1">
       <c r="A212" s="1">
         <v>44773</v>
       </c>
@@ -2353,7 +2615,7 @@
         <v>13.17</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" ht="15.75" customHeight="1">
       <c r="A213" s="1">
         <v>44804</v>
       </c>
@@ -2361,7 +2623,7 @@
         <v>13.08</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" ht="15.75" customHeight="1">
       <c r="A214" s="1" t="s">
         <v>92</v>
       </c>
@@ -2369,31 +2631,31 @@
         <v>12.57</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" ht="15.75" customHeight="1">
       <c r="A215" s="1">
         <v>44865</v>
       </c>
       <c r="B215" s="4">
-        <v>12.72</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12.720000000000001</v>
+      </c>
+    </row>
+    <row r="216" ht="15.75" customHeight="1">
       <c r="A216" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B216" s="4">
-        <v>12.78</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12.779999999999999</v>
+      </c>
+    </row>
+    <row r="217" ht="15.75" customHeight="1">
       <c r="A217" s="1">
         <v>44926</v>
       </c>
       <c r="B217" s="4">
-        <v>13.38</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13.380000000000001</v>
+      </c>
+    </row>
+    <row r="218" ht="15.75" customHeight="1">
       <c r="A218" s="1">
         <v>44957</v>
       </c>
@@ -2401,15 +2663,15 @@
         <v>12.84</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" ht="15.75" customHeight="1">
       <c r="A219" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B219" s="4">
-        <v>13.2</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13.199999999999999</v>
+      </c>
+    </row>
+    <row r="220" ht="15.75" customHeight="1">
       <c r="A220" s="1">
         <v>45016</v>
       </c>
@@ -2417,15 +2679,15 @@
         <v>11.82</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" ht="15.75" customHeight="1">
       <c r="A221" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B221" s="4">
-        <v>11.97</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>11.970000000000001</v>
+      </c>
+    </row>
+    <row r="222" ht="15.75" customHeight="1">
       <c r="A222" s="1">
         <v>45077</v>
       </c>
@@ -2433,7 +2695,7 @@
         <v>13.74</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" ht="15.75" customHeight="1">
       <c r="A223" s="1" t="s">
         <v>96</v>
       </c>
@@ -2441,7 +2703,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" ht="15.75" customHeight="1">
       <c r="A224" s="1">
         <v>45138</v>
       </c>
@@ -2449,15 +2711,15 @@
         <v>13.77</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" ht="15.75" customHeight="1">
       <c r="A225" s="1">
         <v>45169</v>
       </c>
       <c r="B225" s="4">
-        <v>13.53</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13.529999999999999</v>
+      </c>
+    </row>
+    <row r="226" ht="15.75" customHeight="1">
       <c r="A226" s="1" t="s">
         <v>97</v>
       </c>
@@ -2465,7 +2727,7 @@
         <v>13.41</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" ht="15.75" customHeight="1">
       <c r="A227" s="1">
         <v>45230</v>
       </c>
@@ -2473,7 +2735,7 @@
         <v>13.23</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" ht="15.75" customHeight="1">
       <c r="A228" s="1" t="s">
         <v>98</v>
       </c>
@@ -2481,15 +2743,15 @@
         <v>13.59</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" ht="15.75" customHeight="1">
       <c r="A229" s="1">
         <v>45291</v>
       </c>
       <c r="B229" s="4">
-        <v>14.04</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>14.039999999999999</v>
+      </c>
+    </row>
+    <row r="230" ht="15.75" customHeight="1">
       <c r="A230" s="1">
         <v>45322</v>
       </c>
@@ -2497,7 +2759,7 @@
         <v>13.92</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" ht="15.75" customHeight="1">
       <c r="A231" s="1" t="s">
         <v>99</v>
       </c>
@@ -2505,7 +2767,7 @@
         <v>14.43</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" ht="15.75" customHeight="1">
       <c r="A232" s="1">
         <v>45382</v>
       </c>
@@ -2513,7 +2775,7 @@
         <v>12.66</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" ht="15.75" customHeight="1">
       <c r="A233" s="1" t="s">
         <v>100</v>
       </c>
@@ -2521,15 +2783,15 @@
         <v>13.44</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" ht="15.75" customHeight="1">
       <c r="A234" s="1">
         <v>45443</v>
       </c>
       <c r="B234" s="4">
-        <v>13.14</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13.140000000000001</v>
+      </c>
+    </row>
+    <row r="235" ht="15.75" customHeight="1">
       <c r="A235" s="1" t="s">
         <v>101</v>
       </c>
@@ -2537,7 +2799,7 @@
         <v>13.56</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" ht="15.75" customHeight="1">
       <c r="A236" s="1">
         <v>45504</v>
       </c>
@@ -2545,15 +2807,15 @@
         <v>12.81</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" ht="15.75" customHeight="1">
       <c r="A237" s="1">
         <v>45535</v>
       </c>
       <c r="B237" s="4">
-        <v>13.62</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13.619999999999999</v>
+      </c>
+    </row>
+    <row r="238" ht="15.75" customHeight="1">
       <c r="A238" s="1" t="s">
         <v>102</v>
       </c>
@@ -2561,7 +2823,7 @@
         <v>14.01</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" ht="15.75" customHeight="1">
       <c r="A239" s="1">
         <v>45596</v>
       </c>
@@ -2569,7 +2831,7 @@
         <v>14.19</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" ht="15.75" customHeight="1">
       <c r="A240" s="1" t="s">
         <v>103</v>
       </c>
@@ -2577,7 +2839,7 @@
         <v>14.43</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" ht="15.75" customHeight="1">
       <c r="A241" s="1">
         <v>45657</v>
       </c>
@@ -2585,7 +2847,7 @@
         <v>14.31</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" ht="15.75" customHeight="1">
       <c r="A242" s="1">
         <v>45688</v>
       </c>
@@ -2593,15 +2855,15 @@
         <v>13.83</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" ht="15.75" customHeight="1">
       <c r="A243" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B243" s="4">
-        <v>14.28</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>14.279999999999999</v>
+      </c>
+    </row>
+    <row r="244" ht="15.75" customHeight="1">
       <c r="A244" s="1">
         <v>45747</v>
       </c>
@@ -2609,7 +2871,7 @@
         <v>13.83</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" ht="15.75" customHeight="1">
       <c r="A245" s="1" t="s">
         <v>105</v>
       </c>
@@ -2617,7 +2879,7 @@
         <v>13.41</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" ht="15.75" customHeight="1">
       <c r="A246" s="1">
         <v>45808</v>
       </c>
@@ -2625,7 +2887,7 @@
         <v>14.01</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" ht="15.75" customHeight="1">
       <c r="A247" s="1" t="s">
         <v>106</v>
       </c>
@@ -2633,15 +2895,15 @@
         <v>13.59</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" ht="15.75" customHeight="1">
       <c r="A248" s="1">
         <v>45869</v>
       </c>
       <c r="B248" s="4">
-        <v>13.86</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13.859999999999999</v>
+      </c>
+    </row>
+    <row r="249" ht="15.75" customHeight="1">
       <c r="A249" s="1">
         <v>45900</v>
       </c>
@@ -2649,15 +2911,15 @@
         <v>12.51</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" ht="15.75" customHeight="1">
       <c r="A250" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B250" s="4">
-        <v>13.29</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>13.289999999999999</v>
+      </c>
+    </row>
+    <row r="251" ht="15.75" customHeight="1">
       <c r="A251" s="1">
         <v>45961</v>
       </c>
@@ -2665,7 +2927,7 @@
         <v>12.18</v>
       </c>
     </row>
-    <row r="252" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" ht="15.75" customHeight="1">
       <c r="A252" s="1" t="s">
         <v>108</v>
       </c>
@@ -2673,8 +2935,18 @@
         <v>12</v>
       </c>
     </row>
+    <row r="253" ht="15.75" customHeight="1">
+      <c r="A253" s="1">
+        <v>46022</v>
+      </c>
+      <c r="B253">
+        <v>12.119999999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000008" footer="0.31496062000000008"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157500000008" bottom="0.78740157500000008" header="0.31496062000000014" footer="0.31496062000000014"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>